<commit_message>
Fixes to the sample submission template coord formula, sample submission parent pedigree and validation of sample name for project link.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_vtest.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_vtest.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="U7" authorId="0">
@@ -1675,7 +1675,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.16"/>
@@ -16326,12 +16326,12 @@
       <formula1>Index!$E$2:$E$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
-      <formula1>IF(OR($H13="Tube",$H13="96-well plate"),Index!$A$2:$A$97,IF($H13="384-well plate",Index!$B$2:$B$385,IF(OR($H13="Tube Strip 2x1", $H13="Tube Strip 3x1", $H13="Tube Strip 4x1", $H13="Tube Strip 5x1", $H13="Tube Strip 6x1", $H13="Tube Strip 7x1", $H13="Tube Strip 8x1"),Index!$C$2:$C$9,"")))</formula1>
+    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
+      <formula1>Index!$B$2:$B$385</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
-      <formula1>Index!$B$2:$B$385</formula1>
+    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
+      <formula1>IF($H8="96-well plate",Index!$A$2:$A$97,IF($H8="384-well plate",Index!$B$2:$B$385,IF(OR($H8="Tube Strip 2x1", $H8="Tube Strip 3x1", $H8="Tube Strip 4x1", $H8="Tube Strip 5x1", $H8="Tube Strip 6x1", $H8="Tube Strip 7x1", $H8="Tube Strip 8x1"),Index!$C$2:$C$9,"")))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -16357,7 +16357,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.02"/>

</xml_diff>